<commit_message>
Updated readme, documentation, pkgdown
</commit_message>
<xml_diff>
--- a/docs/reference/TP53_EGFR_in_tissue_cancer.xlsx.xlsx
+++ b/docs/reference/TP53_EGFR_in_tissue_cancer.xlsx.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">ensembl</t>
   </si>
@@ -94,6 +94,39 @@
     <t xml:space="preserve">EGFR</t>
   </si>
   <si>
+    <t xml:space="preserve">cells in basal layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cells in corneal layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cells in spinous layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endothelial cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extracellular matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fibrohistiocytic cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">langerhans cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lymphocytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vascular mural cells</t>
+  </si>
+  <si>
     <t xml:space="preserve">cancer</t>
   </si>
   <si>
@@ -124,12 +157,30 @@
     <t xml:space="preserve">breast cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">2.289e-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">glioma</t>
   </si>
   <si>
+    <t xml:space="preserve">9.953e-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">melanoma</t>
   </si>
   <si>
+    <t xml:space="preserve">2.750e-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.618e-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.079e-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.846e-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">main_location</t>
   </si>
   <si>
@@ -163,10 +214,19 @@
     <t xml:space="preserve">go_id</t>
   </si>
   <si>
+    <t xml:space="preserve">Supported</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nucleoplasm</t>
   </si>
   <si>
-    <t xml:space="preserve">Nucleoplasm (GO:0005654)</t>
+    <t xml:space="preserve">Cytosol;Mitochondria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytosol;Mitochondria;Nucleoplasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytosol (GO:0005829);Mitochondria (GO:0005739);Nucleoplasm (GO:0005654)</t>
   </si>
   <si>
     <t xml:space="preserve">Cell Junctions;Plasma membrane</t>
@@ -181,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -500,12 +560,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -741,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -761,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -781,7 +841,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -858,10 +918,10 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -878,7 +938,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -898,7 +958,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -918,12 +978,152 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
         <v>23</v>
       </c>
       <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -934,12 +1134,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -949,31 +1149,31 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
@@ -984,7 +1184,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -1001,8 +1201,8 @@
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
-      <c r="K2" t="n">
-        <v>0.02289</v>
+      <c r="K2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3">
@@ -1013,7 +1213,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
@@ -1028,8 +1228,8 @@
         <v>7</v>
       </c>
       <c r="H3"/>
-      <c r="I3" t="n">
-        <v>0.09953</v>
+      <c r="I3" t="s">
+        <v>49</v>
       </c>
       <c r="J3"/>
       <c r="K3"/>
@@ -1042,7 +1242,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1059,8 +1259,8 @@
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
-      <c r="K4" t="n">
-        <v>0.0275</v>
+      <c r="K4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5">
@@ -1071,23 +1271,23 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5"/>
-      <c r="I5" t="n">
-        <v>0.02618</v>
+      <c r="I5" t="s">
+        <v>52</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -1100,23 +1300,23 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H6"/>
-      <c r="I6" t="n">
-        <v>0.1079</v>
+      <c r="I6" t="s">
+        <v>53</v>
       </c>
       <c r="J6"/>
       <c r="K6"/>
@@ -1129,25 +1329,25 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
-      <c r="K7" t="n">
-        <v>0.02846</v>
+      <c r="K7" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1157,12 +1357,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1175,37 +1375,37 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="M1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="N1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
@@ -1216,26 +1416,28 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2"/>
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
       <c r="F2"/>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2"/>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">
@@ -1249,14 +1451,14 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -1265,7 +1467,7 @@
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>